<commit_message>
added Zeitaufzeichnung Sprint 9
</commit_message>
<xml_diff>
--- a/organisation/Zeitaufzeichnung.xlsx
+++ b/organisation/Zeitaufzeichnung.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ffce2ed5387dd938/Dokumente/GitHub/cellarius/organisation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jakob\Documents\Jakob\Schule\HTL\SJ2122\SYP\Cellarius\cellarius\organisation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="30" documentId="13_ncr:1_{13ED57DF-28D8-4003-BA6A-E31CD5FEAD83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9AF88412-EC40-4C79-A8E7-15C0CA90E559}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32EBFC4F-E47A-4724-ACE2-02DC030DEF46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4320" yWindow="2880" windowWidth="34170" windowHeight="15345" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Gesamt" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="130">
   <si>
     <t>Jakob Lehner</t>
   </si>
@@ -370,6 +370,66 @@
   </si>
   <si>
     <t>Technologie Research</t>
+  </si>
+  <si>
+    <t>Sprint 8 - Zeitaufzeichnung</t>
+  </si>
+  <si>
+    <t>Sprint 9 - Zeitaufzeichnung</t>
+  </si>
+  <si>
+    <t>GPT-Neo Dockerize</t>
+  </si>
+  <si>
+    <t>MongoDB Leocloud</t>
+  </si>
+  <si>
+    <t>MongoDB Webinterface</t>
+  </si>
+  <si>
+    <t>Beprechnung</t>
+  </si>
+  <si>
+    <t>Präsentation</t>
+  </si>
+  <si>
+    <t>Kube</t>
+  </si>
+  <si>
+    <t>Packages</t>
+  </si>
+  <si>
+    <t>Virtualisierung - minikube &amp; LeoCloud</t>
+  </si>
+  <si>
+    <t>Actions</t>
+  </si>
+  <si>
+    <t>Aufsetzen mit Beeyond</t>
+  </si>
+  <si>
+    <t>GPT-Neo Script (Text Generation)</t>
+  </si>
+  <si>
+    <t>Pythonscript für Import dockerisieren</t>
+  </si>
+  <si>
+    <t>Docker Leocloud init</t>
+  </si>
+  <si>
+    <t>Martin Hausleitner, Romeo Bhuiyan</t>
+  </si>
+  <si>
+    <t>Martin Hausleitner, Romeo Bhuiyan, Zeno Paukner, Jakob Lehner</t>
+  </si>
+  <si>
+    <t>Martin Hausleitner, Zeno Paukner, Jakob Lehner</t>
+  </si>
+  <si>
+    <t>Zeno Paukner, Martin Hausleitner</t>
+  </si>
+  <si>
+    <t>Martin Hausleitner, Jakob Lehner</t>
   </si>
 </sst>
 </file>
@@ -380,7 +440,7 @@
     <numFmt numFmtId="164" formatCode="[h]:mm"/>
     <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -429,6 +489,17 @@
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Roboto"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -498,7 +569,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -567,6 +638,9 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="20" fontId="7" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1013,6 +1087,59 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="6605042" cy="897724"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Grafik 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FF5C03D9-427C-46FC-A051-0BF7734F2C56}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="6605042" cy="897724"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1620,15 +1747,273 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D40A83D3-A6B2-4115-B045-06746A406E46}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P29" sqref="P29"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="47.42578125" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="60.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A3" s="8" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="37" t="s">
+        <v>112</v>
+      </c>
+      <c r="B5" s="32"/>
+      <c r="C5" s="37" t="s">
+        <v>125</v>
+      </c>
+      <c r="D5" s="38">
+        <v>0.4513888888888889</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="37" t="s">
+        <v>113</v>
+      </c>
+      <c r="B6" s="32"/>
+      <c r="C6" s="37" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" s="38">
+        <v>6.25E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="37" t="s">
+        <v>114</v>
+      </c>
+      <c r="B7" s="32"/>
+      <c r="C7" s="37" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="38">
+        <v>2.0833333333333332E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="37" t="s">
+        <v>115</v>
+      </c>
+      <c r="B8" s="32"/>
+      <c r="C8" s="37" t="s">
+        <v>126</v>
+      </c>
+      <c r="D8" s="38">
+        <v>0.20833333333333334</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="37" t="s">
+        <v>116</v>
+      </c>
+      <c r="B9" s="32"/>
+      <c r="C9" s="37" t="s">
+        <v>127</v>
+      </c>
+      <c r="D9" s="38">
+        <v>2.0833333333333332E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="37" t="s">
+        <v>117</v>
+      </c>
+      <c r="B10" s="32"/>
+      <c r="C10" s="37" t="s">
+        <v>128</v>
+      </c>
+      <c r="D10" s="38">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="37" t="s">
+        <v>59</v>
+      </c>
+      <c r="B11" s="32"/>
+      <c r="C11" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="D11" s="38">
+        <v>2.0833333333333332E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="37" t="s">
+        <v>118</v>
+      </c>
+      <c r="B12" s="32"/>
+      <c r="C12" s="37" t="s">
+        <v>87</v>
+      </c>
+      <c r="D12" s="38">
+        <v>0.16666666666666666</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="37" t="s">
+        <v>119</v>
+      </c>
+      <c r="B13" s="32"/>
+      <c r="C13" s="37" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13" s="38">
+        <v>0.2638888888888889</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="37" t="s">
+        <v>120</v>
+      </c>
+      <c r="C14" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="D14" s="38">
+        <v>0.27083333333333331</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="37" t="s">
+        <v>121</v>
+      </c>
+      <c r="C15" s="37" t="s">
+        <v>90</v>
+      </c>
+      <c r="D15" s="38">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="37" t="s">
+        <v>122</v>
+      </c>
+      <c r="C16" s="37" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" s="38">
+        <v>0.40972222222222227</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="37" t="s">
+        <v>123</v>
+      </c>
+      <c r="C17" s="37" t="s">
+        <v>1</v>
+      </c>
+      <c r="D17" s="38">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="37" t="s">
+        <v>124</v>
+      </c>
+      <c r="C18" s="37" t="s">
+        <v>129</v>
+      </c>
+      <c r="D18" s="38">
+        <v>8.3333333333333329E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C19" s="36"/>
+    </row>
+    <row r="20" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="26" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B21" s="6">
+        <f>D8+D9+D10+D12+D13+D15</f>
+        <v>1.0347222222222223</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B22" s="6">
+        <f>D5+D8+D16</f>
+        <v>1.0694444444444444</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23" s="6">
+        <f>D5+D7+D8+D6+D9+D10+D17+D18</f>
+        <v>1.3472222222222221</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B24" s="6">
+        <f>D8+D9+D11+D12+D14+D15+D18</f>
+        <v>0.89583333333333337</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="B25" s="24">
+        <f>SUM(B21:B24)</f>
+        <v>4.3472222222222223</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -3079,7 +3464,7 @@
   <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3097,7 +3482,7 @@
     <row r="2" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Clean up time sheetsg
</commit_message>
<xml_diff>
--- a/organisation/Zeitaufzeichnung.xlsx
+++ b/organisation/Zeitaufzeichnung.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zenop\Documents\_SYP\cellarius\organisation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2D62A11-D71B-4494-91FF-B64203D44730}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D779874-9CE2-4F3B-9E37-2F040B4BE19F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Gesamt" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="139">
   <si>
     <t>Jakob Lehner</t>
   </si>
@@ -427,6 +427,36 @@
   </si>
   <si>
     <t>Sprint 8 - Zeitaufzeichnung</t>
+  </si>
+  <si>
+    <t>Sprint 9</t>
+  </si>
+  <si>
+    <t>Sprint 10</t>
+  </si>
+  <si>
+    <t>Sprint 11</t>
+  </si>
+  <si>
+    <t>Sprint 12</t>
+  </si>
+  <si>
+    <t>Sprint 13</t>
+  </si>
+  <si>
+    <t>Sprint 14</t>
+  </si>
+  <si>
+    <t>Sprint 15</t>
+  </si>
+  <si>
+    <t>Sprint 16</t>
+  </si>
+  <si>
+    <t>Protokollierung Email auslesen</t>
+  </si>
+  <si>
+    <t>Protokollierung Emailauswertung</t>
   </si>
 </sst>
 </file>
@@ -555,15 +585,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -579,9 +605,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -696,6 +719,59 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing10.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="6605042" cy="897724"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Grafik 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{79FAB531-021C-4334-AD4D-CBA89F4BDF4E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="6605042" cy="897724"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -973,13 +1049,13 @@
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="6605042" cy="897724"/>
+    <xdr:ext cx="6607341" cy="899695"/>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="2" name="Grafik 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E8D9FCE6-83DA-4CBD-A2D5-BC9A0B587E90}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{11F533DB-5AB2-47BA-91C5-167608F6E06A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1005,7 +1081,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="6605042" cy="897724"/>
+          <a:ext cx="6607341" cy="899695"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1032,7 +1108,7 @@
         <xdr:cNvPr id="2" name="Grafik 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A54653A1-5C65-4C36-AD82-39211B2E0F9E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E8D9FCE6-83DA-4CBD-A2D5-BC9A0B587E90}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1085,7 +1161,7 @@
         <xdr:cNvPr id="2" name="Grafik 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{79FAB531-021C-4334-AD4D-CBA89F4BDF4E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A54653A1-5C65-4C36-AD82-39211B2E0F9E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1412,57 +1488,57 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.85546875" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" style="14" customWidth="1"/>
-    <col min="3" max="3" width="17.28515625" style="15" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" style="14" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" style="14" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" style="11" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" style="12" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" style="11" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" style="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="7" customFormat="1" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="9"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-    </row>
-    <row r="2" spans="1:7" s="7" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="9"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-    </row>
-    <row r="3" spans="1:7" s="7" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="8" t="s">
+    <row r="1" spans="1:7" s="5" customFormat="1" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="7"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+    </row>
+    <row r="2" spans="1:7" s="5" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="7"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+    </row>
+    <row r="3" spans="1:7" s="5" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="E4" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="F4" s="19" t="s">
+      <c r="F4" s="16" t="s">
         <v>16</v>
       </c>
       <c r="G4" s="1"/>
@@ -1471,250 +1547,367 @@
       <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="12">
+      <c r="B5" s="10">
         <v>0.3125</v>
       </c>
-      <c r="C5" s="12">
+      <c r="C5" s="10">
         <v>0.61944444444444446</v>
       </c>
-      <c r="D5" s="12">
+      <c r="D5" s="10">
         <v>0.3125</v>
       </c>
-      <c r="E5" s="12">
+      <c r="E5" s="10">
         <v>0.3125</v>
       </c>
-      <c r="F5" s="20">
+      <c r="F5" s="17">
         <f>SUM(B5,C5,D5,E5)</f>
         <v>1.5569444444444445</v>
       </c>
-      <c r="G5" s="18"/>
+      <c r="G5" s="15"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="12">
+      <c r="B6" s="10">
         <v>1.09375</v>
       </c>
-      <c r="C6" s="12">
+      <c r="C6" s="10">
         <v>1.09375</v>
       </c>
-      <c r="D6" s="12">
+      <c r="D6" s="10">
         <v>1.09375</v>
       </c>
-      <c r="E6" s="12">
+      <c r="E6" s="10">
         <v>1.09375</v>
       </c>
-      <c r="F6" s="20">
-        <f t="shared" ref="F6:F15" si="0">SUM(B6,C6,D6,E6)</f>
+      <c r="F6" s="17">
+        <f>SUM(B6,C6,D6,E6)</f>
         <v>4.375</v>
       </c>
-      <c r="G6" s="18"/>
+      <c r="G6" s="15"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="12">
+      <c r="B7" s="10">
         <v>0.25</v>
       </c>
-      <c r="C7" s="12">
+      <c r="C7" s="10">
         <v>0.3888888888888889</v>
       </c>
-      <c r="D7" s="12">
+      <c r="D7" s="10">
         <v>0.25</v>
       </c>
-      <c r="E7" s="12">
+      <c r="E7" s="10">
         <v>0.25</v>
       </c>
-      <c r="F7" s="20">
-        <f t="shared" si="0"/>
+      <c r="F7" s="17">
+        <f t="shared" ref="F7:F22" si="0">SUM(B7,C7,D7,E7)</f>
         <v>1.1388888888888888</v>
       </c>
-      <c r="G7" s="18"/>
+      <c r="G7" s="15"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="12">
+      <c r="B8" s="10">
         <v>0.60416666666666663</v>
       </c>
-      <c r="C8" s="12">
+      <c r="C8" s="10">
         <v>1.0215277777777778</v>
       </c>
-      <c r="D8" s="12">
+      <c r="D8" s="10">
         <v>0.66666666666666663</v>
       </c>
-      <c r="E8" s="12">
+      <c r="E8" s="10">
         <v>0.59097222222222223</v>
       </c>
-      <c r="F8" s="20">
+      <c r="F8" s="17">
         <f t="shared" si="0"/>
         <v>2.8833333333333333</v>
       </c>
-      <c r="G8" s="18"/>
+      <c r="G8" s="15"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="12">
+      <c r="B9" s="10">
         <v>1.0451388888888888</v>
       </c>
-      <c r="C9" s="12">
+      <c r="C9" s="10">
         <v>1.1416666666666666</v>
       </c>
-      <c r="D9" s="12">
+      <c r="D9" s="10">
         <v>1.0541666666666667</v>
       </c>
-      <c r="E9" s="12">
+      <c r="E9" s="10">
         <v>0.7729166666666667</v>
       </c>
-      <c r="F9" s="20">
+      <c r="F9" s="17">
         <f t="shared" si="0"/>
         <v>4.0138888888888893</v>
       </c>
-      <c r="G9" s="18"/>
+      <c r="G9" s="15"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="22">
+      <c r="B10" s="19">
         <v>0.35694444444444445</v>
       </c>
-      <c r="C10" s="12">
+      <c r="C10" s="10">
         <v>0.50069444444444444</v>
       </c>
-      <c r="D10" s="15">
+      <c r="D10" s="12">
         <v>0.48541666666666666</v>
       </c>
-      <c r="E10" s="15">
+      <c r="E10" s="12">
         <v>0.34791666666666665</v>
       </c>
-      <c r="F10" s="20">
+      <c r="F10" s="17">
         <f t="shared" si="0"/>
         <v>1.6909722222222221</v>
       </c>
-      <c r="G10" s="18"/>
+      <c r="G10" s="15"/>
     </row>
     <row r="11" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="6">
+      <c r="B11" s="4">
         <v>0.4770833333333333</v>
       </c>
-      <c r="C11" s="12">
+      <c r="C11" s="10">
         <v>0.33333333333333331</v>
       </c>
-      <c r="D11" s="15">
+      <c r="D11" s="12">
         <v>0.16666666666666666</v>
       </c>
-      <c r="E11" s="15">
+      <c r="E11" s="12">
         <v>0.4770833333333333</v>
       </c>
-      <c r="F11" s="20">
+      <c r="F11" s="17">
         <f t="shared" si="0"/>
         <v>1.4541666666666666</v>
       </c>
-      <c r="G11" s="18"/>
+      <c r="G11" s="15"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="13"/>
-      <c r="C12" s="12"/>
-      <c r="F12" s="20">
+      <c r="B12" s="12">
+        <v>0.80902777777777779</v>
+      </c>
+      <c r="C12" s="12">
+        <v>0.79513888888888884</v>
+      </c>
+      <c r="D12" s="12">
+        <v>0.375</v>
+      </c>
+      <c r="E12" s="12">
+        <v>0.64861111111111114</v>
+      </c>
+      <c r="F12" s="17">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G12" s="18"/>
+        <v>2.6277777777777778</v>
+      </c>
+      <c r="G12" s="15"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="12"/>
-      <c r="F13" s="20">
+      <c r="B13" s="19">
+        <v>0.57500000000000007</v>
+      </c>
+      <c r="C13" s="10">
+        <v>0.53888888888888886</v>
+      </c>
+      <c r="D13" s="12">
+        <v>0.57500000000000007</v>
+      </c>
+      <c r="E13" s="12">
+        <v>0.58888888888888891</v>
+      </c>
+      <c r="F13" s="17">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G13" s="18"/>
+        <v>2.2777777777777781</v>
+      </c>
+      <c r="G13" s="15"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F14" s="20">
+      <c r="B14" s="12">
+        <v>0.58958333333333335</v>
+      </c>
+      <c r="C14" s="12">
+        <v>0.57847222222222217</v>
+      </c>
+      <c r="D14" s="12">
+        <v>0.74930555555555556</v>
+      </c>
+      <c r="E14" s="12">
+        <v>0.59236111111111112</v>
+      </c>
+      <c r="F14" s="17">
+        <f t="shared" si="0"/>
+        <v>2.509722222222222</v>
+      </c>
+      <c r="G14" s="15"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B15" s="10">
+        <v>1.2916666666666667</v>
+      </c>
+      <c r="C15" s="10">
+        <v>1.2013888888888888</v>
+      </c>
+      <c r="D15" s="10">
+        <v>1.4722222222222223</v>
+      </c>
+      <c r="E15" s="10">
+        <v>1.1041666666666667</v>
+      </c>
+      <c r="F15" s="17">
+        <f t="shared" si="0"/>
+        <v>5.0694444444444446</v>
+      </c>
+      <c r="G15" s="15"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B16" s="10"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="17">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G14" s="18"/>
-    </row>
-    <row r="15" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="16"/>
-      <c r="B15" s="17">
-        <f>SUM(B5,B7,B6,B8,B9,B10,B11,B12,B13,B14)</f>
-        <v>4.1395833333333325</v>
-      </c>
-      <c r="C15" s="17">
-        <f>SUM(C5,C6,C7,C8,C9,C10,C11,C12,C13,C14)</f>
-        <v>5.0993055555555546</v>
-      </c>
-      <c r="D15" s="17">
-        <f>SUM(D5:D14)</f>
-        <v>4.0291666666666668</v>
-      </c>
-      <c r="E15" s="17">
-        <f>SUM(E5:E14)</f>
-        <v>3.8451388888888887</v>
-      </c>
-      <c r="F15" s="21">
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B17" s="10"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="17">
         <f t="shared" si="0"/>
-        <v>17.113194444444442</v>
-      </c>
-      <c r="G15" s="18"/>
-    </row>
-    <row r="16" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="18" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="4"/>
-      <c r="B18" s="5"/>
-    </row>
-    <row r="19" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="3"/>
-      <c r="B19" s="6"/>
-    </row>
-    <row r="20" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="3"/>
-      <c r="B20" s="6"/>
-    </row>
-    <row r="21" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="6"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-    </row>
-    <row r="22" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="6"/>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-    </row>
-    <row r="23" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="6"/>
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
-    </row>
-    <row r="24" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="6"/>
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
-    </row>
-    <row r="25" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="6"/>
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B18" s="10"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B19" s="10"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B20" s="10"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B21" s="10"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B22" s="10"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="13"/>
+      <c r="B23" s="14">
+        <f>SUM(B5:B22)</f>
+        <v>7.4048611111111109</v>
+      </c>
+      <c r="C23" s="14">
+        <f t="shared" ref="C23:E23" si="1">SUM(C5:C22)</f>
+        <v>8.2131944444444436</v>
+      </c>
+      <c r="D23" s="14">
+        <f t="shared" si="1"/>
+        <v>7.2006944444444452</v>
+      </c>
+      <c r="E23" s="14">
+        <f t="shared" si="1"/>
+        <v>6.7791666666666659</v>
+      </c>
+      <c r="F23" s="18">
+        <f>SUM(B23,C23,D23,E23)</f>
+        <v>29.597916666666663</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="4"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+    </row>
+    <row r="25" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="4"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
@@ -1732,8 +1925,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D40A83D3-A6B2-4115-B045-06746A406E46}">
   <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" activeCellId="1" sqref="K23 J4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1745,7 +1938,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="66.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="6" t="s">
         <v>127</v>
       </c>
     </row>
@@ -1767,7 +1960,7 @@
       <c r="B5" t="s">
         <v>125</v>
       </c>
-      <c r="C5" s="23">
+      <c r="C5" s="20">
         <v>0.4513888888888889</v>
       </c>
     </row>
@@ -1778,7 +1971,7 @@
       <c r="B6" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="23">
+      <c r="C6" s="20">
         <v>6.25E-2</v>
       </c>
     </row>
@@ -1789,7 +1982,7 @@
       <c r="B7" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="23">
+      <c r="C7" s="20">
         <v>2.0833333333333332E-2</v>
       </c>
     </row>
@@ -1800,7 +1993,7 @@
       <c r="B8" t="s">
         <v>101</v>
       </c>
-      <c r="C8" s="23">
+      <c r="C8" s="20">
         <v>0.33333333333333331</v>
       </c>
     </row>
@@ -1811,7 +2004,7 @@
       <c r="B9" t="s">
         <v>98</v>
       </c>
-      <c r="C9" s="23">
+      <c r="C9" s="20">
         <v>2.0833333333333332E-2</v>
       </c>
     </row>
@@ -1822,98 +2015,98 @@
       <c r="B10" t="s">
         <v>126</v>
       </c>
-      <c r="C10" s="23">
+      <c r="C10" s="20">
         <v>0.25</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="31" t="s">
+      <c r="A11" s="28" t="s">
         <v>59</v>
       </c>
       <c r="B11" t="s">
         <v>0</v>
       </c>
-      <c r="C11" s="23">
+      <c r="C11" s="20">
         <v>2.0833333333333332E-2</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="31" t="s">
+      <c r="A12" s="28" t="s">
         <v>116</v>
       </c>
-      <c r="B12" s="32" t="s">
+      <c r="B12" s="29" t="s">
         <v>87</v>
       </c>
-      <c r="C12" s="23">
+      <c r="C12" s="20">
         <v>0.16666666666666666</v>
       </c>
-      <c r="D12" s="23"/>
-      <c r="E12" s="23"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="20"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="31" t="s">
+      <c r="A13" s="28" t="s">
         <v>117</v>
       </c>
-      <c r="B13" s="32" t="s">
+      <c r="B13" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="C13" s="23">
+      <c r="C13" s="20">
         <v>0.2638888888888889</v>
       </c>
-      <c r="D13" s="23"/>
+      <c r="D13" s="20"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="31" t="s">
+      <c r="A14" s="28" t="s">
         <v>118</v>
       </c>
       <c r="B14" t="s">
         <v>0</v>
       </c>
-      <c r="C14" s="23">
+      <c r="C14" s="20">
         <v>0.27083333333333331</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="31" t="s">
+      <c r="A15" s="28" t="s">
         <v>119</v>
       </c>
       <c r="B15" t="s">
         <v>87</v>
       </c>
-      <c r="C15" s="23">
+      <c r="C15" s="20">
         <v>0.29166666666666669</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="31" t="s">
+      <c r="A16" s="28" t="s">
         <v>120</v>
       </c>
       <c r="B16" t="s">
         <v>2</v>
       </c>
-      <c r="C16" s="23">
+      <c r="C16" s="20">
         <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="31" t="s">
+      <c r="A17" s="28" t="s">
         <v>121</v>
       </c>
       <c r="B17" t="s">
         <v>1</v>
       </c>
-      <c r="C17" s="23">
+      <c r="C17" s="20">
         <v>0.25</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="31" t="s">
+      <c r="A18" s="28" t="s">
         <v>122</v>
       </c>
       <c r="B18" t="s">
         <v>1</v>
       </c>
-      <c r="C18" s="23">
+      <c r="C18" s="20">
         <v>8.3333333333333329E-2</v>
       </c>
     </row>
@@ -1924,7 +2117,7 @@
       <c r="B19" t="s">
         <v>3</v>
       </c>
-      <c r="C19" s="23">
+      <c r="C19" s="20">
         <v>6.25E-2</v>
       </c>
     </row>
@@ -1935,15 +2128,15 @@
       <c r="B20" t="s">
         <v>3</v>
       </c>
-      <c r="C20" s="23">
+      <c r="C20" s="20">
         <v>0.16666666666666666</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="27" t="s">
+      <c r="A24" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="B24" s="26" t="s">
+      <c r="B24" s="23" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1951,7 +2144,7 @@
       <c r="A25" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B25" s="6">
+      <c r="B25" s="4">
         <f>C8+C9+C10+C12+C15+C19+C20</f>
         <v>1.2916666666666667</v>
       </c>
@@ -1960,7 +2153,7 @@
       <c r="A26" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B26" s="6">
+      <c r="B26" s="4">
         <f>C5+C8+C16</f>
         <v>1.2013888888888888</v>
       </c>
@@ -1969,7 +2162,7 @@
       <c r="A27" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B27" s="6">
+      <c r="B27" s="4">
         <f>C5+C6+C7+C8+C9+C10+C17+C18</f>
         <v>1.4722222222222221</v>
       </c>
@@ -1978,16 +2171,16 @@
       <c r="A28" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="6">
+      <c r="B28" s="4">
         <f>C8+C9+C12+C11+C14+C15</f>
         <v>1.1041666666666667</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="25" t="s">
+      <c r="A29" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="B29" s="24">
+      <c r="B29" s="21">
         <f>SUM(B25:B28)</f>
         <v>5.0694444444444446</v>
       </c>
@@ -2012,20 +2205,20 @@
     <col min="1" max="1" width="54.140625" customWidth="1"/>
     <col min="2" max="2" width="12.5703125" customWidth="1"/>
     <col min="3" max="3" width="23" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="23"/>
+    <col min="4" max="4" width="9.140625" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="34" customFormat="1" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D1" s="35"/>
-    </row>
-    <row r="2" spans="1:4" s="7" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D2" s="29"/>
-    </row>
-    <row r="3" spans="1:4" s="7" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="8" t="s">
+    <row r="1" spans="1:4" s="31" customFormat="1" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D1" s="32"/>
+    </row>
+    <row r="2" spans="1:4" s="5" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D2" s="26"/>
+    </row>
+    <row r="3" spans="1:4" s="5" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="D3" s="29"/>
+      <c r="D3" s="26"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -2051,7 +2244,7 @@
       <c r="C5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="28">
+      <c r="D5" s="25">
         <v>5.5555555555555552E-2</v>
       </c>
     </row>
@@ -2065,7 +2258,7 @@
       <c r="C6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="28">
+      <c r="D6" s="25">
         <v>8.3333333333333329E-2</v>
       </c>
     </row>
@@ -2079,7 +2272,7 @@
       <c r="C7" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D7" s="28">
+      <c r="D7" s="25">
         <v>8.3333333333333329E-2</v>
       </c>
     </row>
@@ -2093,7 +2286,7 @@
       <c r="C8" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="28">
+      <c r="D8" s="25">
         <v>8.3333333333333329E-2</v>
       </c>
     </row>
@@ -2107,7 +2300,7 @@
       <c r="C9" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="28">
+      <c r="D9" s="25">
         <v>0.20833333333333334</v>
       </c>
     </row>
@@ -2121,7 +2314,7 @@
       <c r="C10" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D10" s="28">
+      <c r="D10" s="25">
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
@@ -2135,7 +2328,7 @@
       <c r="C11" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D11" s="28">
+      <c r="D11" s="25">
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
@@ -2149,7 +2342,7 @@
       <c r="C12" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D12" s="28">
+      <c r="D12" s="25">
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
@@ -2163,15 +2356,15 @@
       <c r="C13" t="s">
         <v>20</v>
       </c>
-      <c r="D13" s="28">
+      <c r="D13" s="25">
         <v>0.125</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="27" t="s">
+      <c r="A18" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="26" t="s">
+      <c r="B18" s="23" t="s">
         <v>18</v>
       </c>
     </row>
@@ -2179,7 +2372,7 @@
       <c r="A19" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B19" s="6">
+      <c r="B19" s="4">
         <f>D6+D10+D13</f>
         <v>0.25</v>
       </c>
@@ -2188,7 +2381,7 @@
       <c r="A20" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B20" s="6">
+      <c r="B20" s="4">
         <f>D6+D10+D13</f>
         <v>0.25</v>
       </c>
@@ -2197,7 +2390,7 @@
       <c r="A21" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B21" s="6">
+      <c r="B21" s="4">
         <f>D5+D9+D13</f>
         <v>0.3888888888888889</v>
       </c>
@@ -2206,16 +2399,16 @@
       <c r="A22" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B22" s="6">
+      <c r="B22" s="4">
         <f>D7+D11+D13</f>
         <v>0.25</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="25" t="s">
+      <c r="A23" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="B23" s="24">
+      <c r="B23" s="21">
         <f>SUM(B19:B22)</f>
         <v>1.1388888888888888</v>
       </c>
@@ -2242,20 +2435,20 @@
     <col min="1" max="1" width="54.140625" customWidth="1"/>
     <col min="2" max="2" width="12.5703125" customWidth="1"/>
     <col min="3" max="3" width="23" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="23"/>
+    <col min="4" max="4" width="9.140625" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="7" customFormat="1" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D1" s="29"/>
-    </row>
-    <row r="2" spans="1:4" s="7" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D2" s="29"/>
-    </row>
-    <row r="3" spans="1:4" s="7" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="8" t="s">
+    <row r="1" spans="1:4" s="5" customFormat="1" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D1" s="26"/>
+    </row>
+    <row r="2" spans="1:4" s="5" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D2" s="26"/>
+    </row>
+    <row r="3" spans="1:4" s="5" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="D3" s="29"/>
+      <c r="D3" s="26"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -2281,7 +2474,7 @@
       <c r="C5" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="30">
+      <c r="D5" s="27">
         <v>1.3888888888888888E-2</v>
       </c>
     </row>
@@ -2295,7 +2488,7 @@
       <c r="C6" t="s">
         <v>0</v>
       </c>
-      <c r="D6" s="23">
+      <c r="D6" s="20">
         <v>0.30624999999999997</v>
       </c>
     </row>
@@ -2309,7 +2502,7 @@
       <c r="C7" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="30">
+      <c r="D7" s="27">
         <v>0.27083333333333331</v>
       </c>
     </row>
@@ -2323,7 +2516,7 @@
       <c r="C8" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="30">
+      <c r="D8" s="27">
         <v>7.6388888888888895E-2</v>
       </c>
     </row>
@@ -2337,7 +2530,7 @@
       <c r="C9" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="23">
+      <c r="D9" s="20">
         <v>6.25E-2</v>
       </c>
     </row>
@@ -2351,7 +2544,7 @@
       <c r="C10" t="s">
         <v>1</v>
       </c>
-      <c r="D10" s="23">
+      <c r="D10" s="20">
         <v>2.013888888888889E-2</v>
       </c>
     </row>
@@ -2365,7 +2558,7 @@
       <c r="C11" t="s">
         <v>1</v>
       </c>
-      <c r="D11" s="23">
+      <c r="D11" s="20">
         <v>0.56874999999999998</v>
       </c>
     </row>
@@ -2379,7 +2572,7 @@
       <c r="C12" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="23">
+      <c r="D12" s="20">
         <v>2.2916666666666669E-2</v>
       </c>
     </row>
@@ -2393,7 +2586,7 @@
       <c r="C13" t="s">
         <v>2</v>
       </c>
-      <c r="D13" s="23">
+      <c r="D13" s="20">
         <v>0.10416666666666667</v>
       </c>
     </row>
@@ -2407,7 +2600,7 @@
       <c r="C14" t="s">
         <v>2</v>
       </c>
-      <c r="D14" s="23">
+      <c r="D14" s="20">
         <v>0.29166666666666669</v>
       </c>
     </row>
@@ -2421,7 +2614,7 @@
       <c r="C15" t="s">
         <v>3</v>
       </c>
-      <c r="D15" s="23">
+      <c r="D15" s="20">
         <v>1.0416666666666666E-2</v>
       </c>
     </row>
@@ -2435,15 +2628,15 @@
       <c r="C16" t="s">
         <v>3</v>
       </c>
-      <c r="D16" s="23">
+      <c r="D16" s="20">
         <v>0.32291666666666669</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="27" t="s">
+      <c r="A18" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="26" t="s">
+      <c r="B18" s="23" t="s">
         <v>18</v>
       </c>
     </row>
@@ -2451,7 +2644,7 @@
       <c r="A19" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B19" s="6">
+      <c r="B19" s="4">
         <f>D15+D16+D7</f>
         <v>0.60416666666666674</v>
       </c>
@@ -2460,7 +2653,7 @@
       <c r="A20" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B20" s="6">
+      <c r="B20" s="4">
         <f>D7+D13+D14</f>
         <v>0.66666666666666674</v>
       </c>
@@ -2469,7 +2662,7 @@
       <c r="A21" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B21" s="6">
+      <c r="B21" s="4">
         <f>D7+D8+D9+D10+D11+D12</f>
         <v>1.0215277777777778</v>
       </c>
@@ -2478,16 +2671,16 @@
       <c r="A22" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B22" s="6">
+      <c r="B22" s="4">
         <f>D5+D6+D7</f>
         <v>0.59097222222222223</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="25" t="s">
+      <c r="A23" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="B23" s="24">
+      <c r="B23" s="21">
         <f>SUM(B19:B22)</f>
         <v>2.8833333333333333</v>
       </c>
@@ -2522,7 +2715,7 @@
     </row>
     <row r="2" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="6" t="s">
         <v>78</v>
       </c>
     </row>
@@ -2550,7 +2743,7 @@
       <c r="C5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="28">
+      <c r="D5" s="25">
         <v>0.22222222222222221</v>
       </c>
     </row>
@@ -2564,10 +2757,10 @@
       <c r="C6" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="28">
+      <c r="D6" s="25">
         <v>0.31458333333333333</v>
       </c>
-      <c r="E6" s="31"/>
+      <c r="E6" s="28"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -2579,10 +2772,10 @@
       <c r="C7" t="s">
         <v>72</v>
       </c>
-      <c r="D7" s="28">
+      <c r="D7" s="25">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="E7" s="31"/>
+      <c r="E7" s="28"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -2594,10 +2787,10 @@
       <c r="C8" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="28">
+      <c r="D8" s="25">
         <v>0.12708333333333333</v>
       </c>
-      <c r="E8" s="31"/>
+      <c r="E8" s="28"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -2609,10 +2802,10 @@
       <c r="C9" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="28">
+      <c r="D9" s="25">
         <v>0.17083333333333331</v>
       </c>
-      <c r="E9" s="31"/>
+      <c r="E9" s="28"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -2624,10 +2817,10 @@
       <c r="C10" t="s">
         <v>65</v>
       </c>
-      <c r="D10" s="28">
+      <c r="D10" s="25">
         <v>0.20833333333333334</v>
       </c>
-      <c r="E10" s="31"/>
+      <c r="E10" s="28"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -2639,10 +2832,10 @@
       <c r="C11" t="s">
         <v>1</v>
       </c>
-      <c r="D11" s="28">
+      <c r="D11" s="25">
         <v>0.23124999999999998</v>
       </c>
-      <c r="E11" s="31"/>
+      <c r="E11" s="28"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -2654,10 +2847,10 @@
       <c r="C12" t="s">
         <v>2</v>
       </c>
-      <c r="D12" s="28">
+      <c r="D12" s="25">
         <v>0.28125</v>
       </c>
-      <c r="E12" s="31"/>
+      <c r="E12" s="28"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -2669,10 +2862,10 @@
       <c r="C13" t="s">
         <v>0</v>
       </c>
-      <c r="D13" s="28">
+      <c r="D13" s="25">
         <v>0.28541666666666665</v>
       </c>
-      <c r="E13" s="31"/>
+      <c r="E13" s="28"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -2684,10 +2877,10 @@
       <c r="C14" t="s">
         <v>1</v>
       </c>
-      <c r="D14" s="28">
+      <c r="D14" s="25">
         <v>0.10416666666666667</v>
       </c>
-      <c r="E14" s="31"/>
+      <c r="E14" s="28"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -2699,10 +2892,10 @@
       <c r="C15" t="s">
         <v>3</v>
       </c>
-      <c r="D15" s="28">
+      <c r="D15" s="25">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="E15" s="31"/>
+      <c r="E15" s="28"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -2714,10 +2907,10 @@
       <c r="C16" t="s">
         <v>20</v>
       </c>
-      <c r="D16" s="28">
+      <c r="D16" s="25">
         <v>0.27916666666666667</v>
       </c>
-      <c r="E16" s="31"/>
+      <c r="E16" s="28"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
@@ -2729,16 +2922,16 @@
       <c r="C17" t="s">
         <v>2</v>
       </c>
-      <c r="D17" s="28">
+      <c r="D17" s="25">
         <v>0.28541666666666665</v>
       </c>
-      <c r="E17" s="31"/>
+      <c r="E17" s="28"/>
     </row>
     <row r="19" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="27" t="s">
+      <c r="A19" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="26" t="s">
+      <c r="B19" s="23" t="s">
         <v>18</v>
       </c>
     </row>
@@ -2746,7 +2939,7 @@
       <c r="A20" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="6">
+      <c r="B20" s="4">
         <f>D5+D6+D7+D10+D16</f>
         <v>1.0451388888888888</v>
       </c>
@@ -2755,7 +2948,7 @@
       <c r="A21" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B21" s="6">
+      <c r="B21" s="4">
         <f>D10+D16+D17+D12</f>
         <v>1.0541666666666667</v>
       </c>
@@ -2764,7 +2957,7 @@
       <c r="A22" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B22" s="6">
+      <c r="B22" s="4">
         <f>D7+D8+D9+D10+D11+D14+D16</f>
         <v>1.1416666666666666</v>
       </c>
@@ -2773,16 +2966,16 @@
       <c r="A23" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B23" s="6">
+      <c r="B23" s="4">
         <f>D10+D13+D16</f>
         <v>0.7729166666666667</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="25" t="s">
+      <c r="A24" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="B24" s="24">
+      <c r="B24" s="21">
         <f>SUM(B20:B23)</f>
         <v>4.0138888888888893</v>
       </c>
@@ -2818,7 +3011,7 @@
     </row>
     <row r="2" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="6" t="s">
         <v>89</v>
       </c>
     </row>
@@ -2840,134 +3033,134 @@
       <c r="A5" t="s">
         <v>88</v>
       </c>
-      <c r="B5" s="32">
+      <c r="B5" s="29">
         <v>44590</v>
       </c>
       <c r="C5" t="s">
         <v>87</v>
       </c>
-      <c r="D5" s="23">
+      <c r="D5" s="20">
         <v>0.22777777777777777</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="31" t="s">
+      <c r="A6" s="28" t="s">
         <v>86</v>
       </c>
-      <c r="B6" s="32">
+      <c r="B6" s="29">
         <v>44584</v>
       </c>
       <c r="C6" t="s">
         <v>85</v>
       </c>
-      <c r="D6" s="23">
+      <c r="D6" s="20">
         <v>2.6388888888888889E-2</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="31" t="s">
+      <c r="A7" s="28" t="s">
         <v>84</v>
       </c>
-      <c r="B7" s="32">
+      <c r="B7" s="29">
         <v>44587</v>
       </c>
       <c r="C7" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="23">
+      <c r="D7" s="20">
         <v>3.472222222222222E-3</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="31" t="s">
+      <c r="A8" s="28" t="s">
         <v>83</v>
       </c>
-      <c r="B8" s="32">
+      <c r="B8" s="29">
         <v>44578</v>
       </c>
       <c r="C8" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="23">
+      <c r="D8" s="20">
         <v>5.5555555555555558E-3</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="31" t="s">
+      <c r="A9" s="28" t="s">
         <v>82</v>
       </c>
-      <c r="B9" s="32">
+      <c r="B9" s="29">
         <v>44587</v>
       </c>
       <c r="C9" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="23">
+      <c r="D9" s="20">
         <v>0.36527777777777781</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="31" t="s">
+      <c r="A10" s="28" t="s">
         <v>81</v>
       </c>
-      <c r="B10" s="32">
+      <c r="B10" s="29">
         <v>44591</v>
       </c>
       <c r="C10" t="s">
         <v>2</v>
       </c>
-      <c r="D10" s="23">
+      <c r="D10" s="20">
         <v>0.3666666666666667</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="31" t="s">
+      <c r="A11" s="28" t="s">
         <v>59</v>
       </c>
-      <c r="B11" s="32">
+      <c r="B11" s="29">
         <v>44591</v>
       </c>
       <c r="C11" t="s">
         <v>2</v>
       </c>
-      <c r="D11" s="23">
+      <c r="D11" s="20">
         <v>1.3888888888888888E-2</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="31" t="s">
+      <c r="A12" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="32">
+      <c r="B12" s="29">
         <v>44591</v>
       </c>
       <c r="C12" t="s">
         <v>80</v>
       </c>
-      <c r="D12" s="23">
+      <c r="D12" s="20">
         <v>9.375E-2</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="31"/>
+      <c r="A13" s="28"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="31"/>
+      <c r="A14" s="28"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="31"/>
+      <c r="A15" s="28"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="31"/>
+      <c r="A16" s="28"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="31"/>
+      <c r="A17" s="28"/>
     </row>
     <row r="19" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="27" t="s">
+      <c r="A19" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="26" t="s">
+      <c r="B19" s="23" t="s">
         <v>18</v>
       </c>
     </row>
@@ -2975,7 +3168,7 @@
       <c r="A20" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="6">
+      <c r="B20" s="4">
         <f>D5+D7+D6+D8+D12</f>
         <v>0.3569444444444444</v>
       </c>
@@ -2984,7 +3177,7 @@
       <c r="A21" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B21" s="6">
+      <c r="B21" s="4">
         <f>D6+D11+D10+D12</f>
         <v>0.50069444444444444</v>
       </c>
@@ -2993,7 +3186,7 @@
       <c r="A22" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B22" s="6">
+      <c r="B22" s="4">
         <f>D6+D9+D12</f>
         <v>0.48541666666666672</v>
       </c>
@@ -3002,16 +3195,16 @@
       <c r="A23" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B23" s="6">
+      <c r="B23" s="4">
         <f>D5+D6+D12</f>
         <v>0.34791666666666665</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="25" t="s">
+      <c r="A24" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="B24" s="24">
+      <c r="B24" s="21">
         <f>SUM(B20:B23)</f>
         <v>1.6909722222222221</v>
       </c>
@@ -3030,7 +3223,7 @@
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3047,7 +3240,7 @@
     </row>
     <row r="2" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="6" t="s">
         <v>96</v>
       </c>
     </row>
@@ -3069,98 +3262,98 @@
       <c r="A5" t="s">
         <v>95</v>
       </c>
-      <c r="B5" s="32">
+      <c r="B5" s="29">
         <v>44602</v>
       </c>
       <c r="C5" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="23">
+      <c r="D5" s="20">
         <v>0.3125</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="31" t="s">
+      <c r="A6" s="28" t="s">
         <v>94</v>
       </c>
-      <c r="B6" s="32">
+      <c r="B6" s="29">
         <v>44605</v>
       </c>
       <c r="C6" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="23">
+      <c r="D6" s="20">
         <v>2.0833333333333332E-2</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="31" t="s">
+      <c r="A7" s="28" t="s">
         <v>93</v>
       </c>
-      <c r="B7" s="32">
+      <c r="B7" s="29">
         <v>44601</v>
       </c>
       <c r="C7" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="23">
+      <c r="D7" s="20">
         <v>0.16666666666666666</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="31" t="s">
+      <c r="A8" s="28" t="s">
         <v>92</v>
       </c>
-      <c r="B8" s="33" t="s">
+      <c r="B8" s="30" t="s">
         <v>91</v>
       </c>
       <c r="C8" t="s">
         <v>90</v>
       </c>
-      <c r="D8" s="23">
+      <c r="D8" s="20">
         <v>0.4770833333333333</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="31"/>
-      <c r="B9" s="32"/>
-      <c r="D9" s="23"/>
+      <c r="A9" s="28"/>
+      <c r="B9" s="29"/>
+      <c r="D9" s="20"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="31"/>
-      <c r="B10" s="32"/>
-      <c r="D10" s="23"/>
+      <c r="A10" s="28"/>
+      <c r="B10" s="29"/>
+      <c r="D10" s="20"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="31"/>
-      <c r="B11" s="32"/>
-      <c r="D11" s="23"/>
+      <c r="A11" s="28"/>
+      <c r="B11" s="29"/>
+      <c r="D11" s="20"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="31"/>
-      <c r="B12" s="32"/>
-      <c r="D12" s="23"/>
+      <c r="A12" s="28"/>
+      <c r="B12" s="29"/>
+      <c r="D12" s="20"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="31"/>
+      <c r="A13" s="28"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="31"/>
+      <c r="A14" s="28"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="31"/>
+      <c r="A15" s="28"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="31"/>
+      <c r="A16" s="28"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="31"/>
+      <c r="A17" s="28"/>
     </row>
     <row r="19" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="27" t="s">
+      <c r="A19" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="26" t="s">
+      <c r="B19" s="23" t="s">
         <v>18</v>
       </c>
     </row>
@@ -3168,7 +3361,7 @@
       <c r="A20" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="6">
+      <c r="B20" s="4">
         <f>D8</f>
         <v>0.4770833333333333</v>
       </c>
@@ -3177,7 +3370,7 @@
       <c r="A21" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B21" s="6">
+      <c r="B21" s="4">
         <f>D6+D5</f>
         <v>0.33333333333333331</v>
       </c>
@@ -3186,7 +3379,7 @@
       <c r="A22" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B22" s="6">
+      <c r="B22" s="4">
         <f>D7</f>
         <v>0.16666666666666666</v>
       </c>
@@ -3195,16 +3388,16 @@
       <c r="A23" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B23" s="6">
+      <c r="B23" s="4">
         <f>D8</f>
         <v>0.4770833333333333</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="25" t="s">
+      <c r="A24" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="B24" s="24">
+      <c r="B24" s="21">
         <f>SUM(B20:B23)</f>
         <v>1.4541666666666666</v>
       </c>
@@ -3220,13 +3413,185 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29FCD946-51AD-4F41-A995-E7CFD151FD64}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B20" sqref="B20:B23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="55.140625" customWidth="1"/>
+    <col min="2" max="2" width="59.42578125" customWidth="1"/>
+    <col min="3" max="3" width="8.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>137</v>
+      </c>
+      <c r="B5" t="s">
+        <v>87</v>
+      </c>
+      <c r="C5" s="20">
+        <v>0.10069444444444443</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="28" t="s">
+        <v>92</v>
+      </c>
+      <c r="B6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="20">
+        <v>0.37013888888888885</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="20">
+        <v>0.16666666666666666</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" s="20">
+        <v>0.12291666666666667</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="28"/>
+      <c r="B9" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="20">
+        <v>0.5</v>
+      </c>
+      <c r="D9" s="20"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="28" t="s">
+        <v>67</v>
+      </c>
+      <c r="B10" t="s">
+        <v>101</v>
+      </c>
+      <c r="C10" s="20">
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="D10" s="20"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="28" t="s">
+        <v>138</v>
+      </c>
+      <c r="B11" t="s">
+        <v>104</v>
+      </c>
+      <c r="C11" s="20">
+        <v>0.21666666666666667</v>
+      </c>
+      <c r="D11" s="20"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="28"/>
+      <c r="B12" s="29"/>
+      <c r="D12" s="20"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="28"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="28"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="28"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="28"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="28"/>
+    </row>
+    <row r="19" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" s="23" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20" s="4">
+        <f>C10+C9+C5</f>
+        <v>0.80902777777777779</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B21" s="4">
+        <f>C6+C10+C11</f>
+        <v>0.79513888888888884</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B22" s="4">
+        <f>C7+C10</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23" s="4">
+        <f>C5+C8+C11+C10</f>
+        <v>0.64861111111111114</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="B24" s="21">
+        <f>SUM(B20:B23)</f>
+        <v>2.6277777777777778</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3235,7 +3600,7 @@
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3252,7 +3617,7 @@
     </row>
     <row r="2" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="6" t="s">
         <v>103</v>
       </c>
     </row>
@@ -3274,13 +3639,13 @@
       <c r="A5" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="32">
+      <c r="B5" s="29">
         <v>44627</v>
       </c>
       <c r="C5" t="s">
         <v>101</v>
       </c>
-      <c r="D5" s="23">
+      <c r="D5" s="20">
         <v>0.33333333333333331</v>
       </c>
     </row>
@@ -3288,13 +3653,13 @@
       <c r="A6" t="s">
         <v>102</v>
       </c>
-      <c r="B6" s="32">
+      <c r="B6" s="29">
         <v>44627</v>
       </c>
       <c r="C6" t="s">
         <v>101</v>
       </c>
-      <c r="D6" s="23">
+      <c r="D6" s="20">
         <v>4.9999999999999996E-2</v>
       </c>
     </row>
@@ -3302,13 +3667,13 @@
       <c r="A7" t="s">
         <v>100</v>
       </c>
-      <c r="B7" s="32">
+      <c r="B7" s="29">
         <v>44640</v>
       </c>
       <c r="C7" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="23">
+      <c r="D7" s="20">
         <v>0.13333333333333333</v>
       </c>
     </row>
@@ -3316,13 +3681,13 @@
       <c r="A8" t="s">
         <v>99</v>
       </c>
-      <c r="B8" s="32">
+      <c r="B8" s="29">
         <v>44631</v>
       </c>
       <c r="C8" t="s">
         <v>98</v>
       </c>
-      <c r="D8" s="23">
+      <c r="D8" s="20">
         <v>0.19166666666666665</v>
       </c>
     </row>
@@ -3330,60 +3695,60 @@
       <c r="A9" t="s">
         <v>97</v>
       </c>
-      <c r="B9" s="32">
+      <c r="B9" s="29">
         <v>44634</v>
       </c>
       <c r="C9" t="s">
         <v>2</v>
       </c>
-      <c r="D9" s="23">
+      <c r="D9" s="20">
         <v>0.15555555555555556</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="31" t="s">
+      <c r="A10" s="28" t="s">
         <v>59</v>
       </c>
-      <c r="B10" s="32">
+      <c r="B10" s="29">
         <v>44640</v>
       </c>
       <c r="C10" t="s">
         <v>0</v>
       </c>
-      <c r="D10" s="23">
+      <c r="D10" s="20">
         <v>1.3888888888888888E-2</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="31"/>
-      <c r="B11" s="32"/>
-      <c r="D11" s="23"/>
+      <c r="A11" s="28"/>
+      <c r="B11" s="29"/>
+      <c r="D11" s="20"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="31"/>
-      <c r="B12" s="32"/>
-      <c r="D12" s="23"/>
+      <c r="A12" s="28"/>
+      <c r="B12" s="29"/>
+      <c r="D12" s="20"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="31"/>
+      <c r="A13" s="28"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="31"/>
+      <c r="A14" s="28"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="31"/>
+      <c r="A15" s="28"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="31"/>
+      <c r="A16" s="28"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="31"/>
+      <c r="A17" s="28"/>
     </row>
     <row r="19" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="27" t="s">
+      <c r="A19" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="26" t="s">
+      <c r="B19" s="23" t="s">
         <v>18</v>
       </c>
     </row>
@@ -3391,7 +3756,7 @@
       <c r="A20" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="6">
+      <c r="B20" s="4">
         <f>D5+D6+D8</f>
         <v>0.57499999999999996</v>
       </c>
@@ -3400,7 +3765,7 @@
       <c r="A21" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B21" s="6">
+      <c r="B21" s="4">
         <f>D5+D6+D9</f>
         <v>0.53888888888888886</v>
       </c>
@@ -3409,7 +3774,7 @@
       <c r="A22" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B22" s="6">
+      <c r="B22" s="4">
         <f>D5+D6+D8</f>
         <v>0.57499999999999996</v>
       </c>
@@ -3418,16 +3783,16 @@
       <c r="A23" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B23" s="6">
+      <c r="B23" s="4">
         <f>D5+D6+D8+D10</f>
         <v>0.5888888888888888</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="25" t="s">
+      <c r="A24" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="B24" s="24">
+      <c r="B24" s="21">
         <f>SUM(B20:B23)</f>
         <v>2.2777777777777777</v>
       </c>
@@ -3463,7 +3828,7 @@
     </row>
     <row r="2" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="6" t="s">
         <v>128</v>
       </c>
     </row>
@@ -3485,13 +3850,13 @@
       <c r="A5" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="32">
+      <c r="B5" s="29">
         <v>44641</v>
       </c>
       <c r="C5" t="s">
         <v>101</v>
       </c>
-      <c r="D5" s="23">
+      <c r="D5" s="20">
         <v>0.39513888888888887</v>
       </c>
     </row>
@@ -3499,13 +3864,13 @@
       <c r="A6" t="s">
         <v>109</v>
       </c>
-      <c r="B6" s="32">
+      <c r="B6" s="29">
         <v>44641</v>
       </c>
       <c r="C6" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="23">
+      <c r="D6" s="20">
         <v>0.16666666666666666</v>
       </c>
     </row>
@@ -3513,13 +3878,13 @@
       <c r="A7" t="s">
         <v>108</v>
       </c>
-      <c r="B7" s="32">
+      <c r="B7" s="29">
         <v>44643</v>
       </c>
       <c r="C7" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="23">
+      <c r="D7" s="20">
         <v>6.25E-2</v>
       </c>
     </row>
@@ -3527,13 +3892,13 @@
       <c r="A8" t="s">
         <v>107</v>
       </c>
-      <c r="B8" s="32">
+      <c r="B8" s="29">
         <v>44643</v>
       </c>
       <c r="C8" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="23">
+      <c r="D8" s="20">
         <v>0.125</v>
       </c>
     </row>
@@ -3541,13 +3906,13 @@
       <c r="A9" t="s">
         <v>106</v>
       </c>
-      <c r="B9" s="32">
+      <c r="B9" s="29">
         <v>44644</v>
       </c>
       <c r="C9" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="23">
+      <c r="D9" s="20">
         <v>0.19444444444444445</v>
       </c>
     </row>
@@ -3555,60 +3920,60 @@
       <c r="A10" t="s">
         <v>105</v>
       </c>
-      <c r="B10" s="32">
+      <c r="B10" s="29">
         <v>44648</v>
       </c>
       <c r="C10" t="s">
         <v>104</v>
       </c>
-      <c r="D10" s="23">
+      <c r="D10" s="20">
         <v>0.18333333333333335</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="31" t="s">
+      <c r="A11" s="28" t="s">
         <v>59</v>
       </c>
-      <c r="B11" s="32">
+      <c r="B11" s="29">
         <v>44654</v>
       </c>
       <c r="C11" t="s">
         <v>0</v>
       </c>
-      <c r="D11" s="23">
+      <c r="D11" s="20">
         <v>1.3888888888888888E-2</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="31"/>
-      <c r="B12" s="32"/>
-      <c r="D12" s="23"/>
+      <c r="A12" s="28"/>
+      <c r="B12" s="29"/>
+      <c r="D12" s="20"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="31"/>
-      <c r="B13" s="32"/>
-      <c r="D13" s="23"/>
+      <c r="A13" s="28"/>
+      <c r="B13" s="29"/>
+      <c r="D13" s="20"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="31"/>
+      <c r="A14" s="28"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="31"/>
+      <c r="A15" s="28"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="31"/>
+      <c r="A16" s="28"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="31"/>
+      <c r="A17" s="28"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="31"/>
+      <c r="A18" s="28"/>
     </row>
     <row r="20" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="27" t="s">
+      <c r="A20" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="26" t="s">
+      <c r="B20" s="23" t="s">
         <v>18</v>
       </c>
     </row>
@@ -3616,7 +3981,7 @@
       <c r="A21" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B21" s="6">
+      <c r="B21" s="4">
         <f>D5+D9</f>
         <v>0.58958333333333335</v>
       </c>
@@ -3625,7 +3990,7 @@
       <c r="A22" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B22" s="6">
+      <c r="B22" s="4">
         <f>D5+D10</f>
         <v>0.57847222222222228</v>
       </c>
@@ -3634,7 +3999,7 @@
       <c r="A23" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B23" s="6">
+      <c r="B23" s="4">
         <f>D5+D7+D8+D6</f>
         <v>0.74930555555555556</v>
       </c>
@@ -3643,16 +4008,16 @@
       <c r="A24" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B24" s="6">
+      <c r="B24" s="4">
         <f>D5+D10+D11</f>
         <v>0.59236111111111112</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="25" t="s">
+      <c r="A25" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="B25" s="24">
+      <c r="B25" s="21">
         <f>SUM(B21:B24)</f>
         <v>2.509722222222222</v>
       </c>

</xml_diff>